<commit_message>
Changes to enable Colab applications
</commit_message>
<xml_diff>
--- a/ps_params.xlsx
+++ b/ps_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuef-my.sharepoint.com/personal/alauren_uef_fi/Documents/codes/plantation_simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{BD37C9A6-105E-4234-89AE-96DD6AE2F5EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FD43333F-0F49-44FD-9762-20E59458A1BB}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{BD37C9A6-105E-4234-89AE-96DD6AE2F5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B0C6140-CF9A-4F88-A162-7A0F411EA27E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
   <dimension ref="A1:XFC13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1830,7 +1830,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="43">
         <v>1</v>
@@ -2786,7 +2786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -4511,8 +4511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2"/>
@@ -4582,7 +4582,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -4611,7 +4611,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G4">
         <v>0</v>

</xml_diff>